<commit_message>
Matriz de trazabilidad de Requisitos de Información para clases y asociaciones
</commit_message>
<xml_diff>
--- a/documentacion/matriz_de_trazabilidad_RI.xlsx
+++ b/documentacion/matriz_de_trazabilidad_RI.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BCC34A-94AC-4166-B39F-0BCA0324B15B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
   <si>
     <t>Actividad</t>
   </si>
@@ -131,9 +130,6 @@
     <t>envía</t>
   </si>
   <si>
-    <t>facilita</t>
-  </si>
-  <si>
     <t>financia</t>
   </si>
   <si>
@@ -143,18 +139,9 @@
     <t>hace</t>
   </si>
   <si>
-    <t>obtiene</t>
-  </si>
-  <si>
     <t>paga</t>
   </si>
   <si>
-    <t>plantea</t>
-  </si>
-  <si>
-    <t>presenta</t>
-  </si>
-  <si>
     <t>realiza</t>
   </si>
   <si>
@@ -168,12 +155,15 @@
   </si>
   <si>
     <t>valora</t>
+  </si>
+  <si>
+    <t>✔</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -753,8 +743,62 @@
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -762,12 +806,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -783,21 +821,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,19 +848,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -831,61 +866,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -948,7 +938,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -983,7 +973,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1160,354 +1150,415 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="9" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="37"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="39"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="39"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="39"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="39"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="39"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="39"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="39"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="39"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="39"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="39"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="39"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="4" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="39"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="39"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="4" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="39"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="4" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="39"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="39"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="39"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="39"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="6" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="39"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="8" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A3:B3"/>
@@ -1522,6 +1573,21 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1529,330 +1595,299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E6D81E-B619-414D-89E6-D5FE91CA84C2}">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="25" t="s">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="37"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="38"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="39"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="39"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="39"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="39"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="39"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="39"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="39"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="39"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="33" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="39"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="39"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="4" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="39"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="39"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="39"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="25"/>
+      <c r="C17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="39"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="39"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="39"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="39"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="40"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
+  <mergeCells count="24">
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
@@ -1866,6 +1901,17 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Matriz de trazabilidad de restricciones
</commit_message>
<xml_diff>
--- a/documentacion/matriz_de_trazabilidad_RI.xlsx
+++ b/documentacion/matriz_de_trazabilidad_RI.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17139420-B4FE-4BB5-B57B-99784BF7AFE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
   <si>
     <t>Actividad</t>
   </si>
@@ -158,12 +159,15 @@
   </si>
   <si>
     <t>✔</t>
+  </si>
+  <si>
+    <t>C                           RI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -794,17 +798,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -817,36 +851,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1150,69 +1154,69 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="9" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1233,11 +1237,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="13"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1246,11 +1250,11 @@
       <c r="H4" s="6"/>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="14" t="s">
         <v>45</v>
       </c>
@@ -1265,11 +1269,11 @@
       </c>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="14" t="s">
         <v>45</v>
       </c>
@@ -1284,11 +1288,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1299,11 +1303,11 @@
       <c r="H7" s="6"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1314,11 +1318,11 @@
       <c r="H8" s="6"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1329,11 +1333,11 @@
       <c r="H9" s="6"/>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1342,11 +1346,11 @@
       <c r="H10" s="6"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
@@ -1357,11 +1361,11 @@
       <c r="H11" s="6"/>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1370,11 +1374,11 @@
       <c r="H12" s="6"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1383,11 +1387,11 @@
       <c r="H13" s="6"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="s">
         <v>45</v>
@@ -1402,11 +1406,11 @@
       </c>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
@@ -1417,11 +1421,11 @@
       <c r="H15" s="6"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="5" t="s">
         <v>45</v>
       </c>
@@ -1436,11 +1440,11 @@
       </c>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1451,11 +1455,11 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1466,11 +1470,11 @@
       <c r="H18" s="6"/>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
@@ -1485,11 +1489,11 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5" t="s">
         <v>45</v>
       </c>
@@ -1504,11 +1508,11 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="21"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6" t="s">
         <v>45</v>
@@ -1521,11 +1525,11 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
@@ -1538,11 +1542,11 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="25"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="15" t="s">
         <v>45</v>
       </c>
@@ -1559,6 +1563,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A3:B3"/>
@@ -1575,19 +1592,6 @@
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1595,18 +1599,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="38" t="s">
@@ -1631,7 +1635,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44"/>
       <c r="B2" s="45"/>
       <c r="C2" s="39"/>
@@ -1642,7 +1646,7 @@
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>29</v>
       </c>
@@ -1657,11 +1661,11 @@
       <c r="H3" s="2"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
         <v>45</v>
@@ -1672,11 +1676,11 @@
       <c r="H4" s="4"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1687,11 +1691,11 @@
       <c r="H5" s="6"/>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="5" t="s">
         <v>45</v>
       </c>
@@ -1706,11 +1710,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1721,11 +1725,11 @@
       <c r="H7" s="6"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1736,11 +1740,11 @@
       </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1749,11 +1753,11 @@
       <c r="H9" s="6"/>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
@@ -1764,11 +1768,11 @@
       <c r="H10" s="6"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1777,7 +1781,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>38</v>
       </c>
@@ -1792,11 +1796,11 @@
       <c r="H12" s="6"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1805,11 +1809,11 @@
       <c r="H13" s="6"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="s">
         <v>45</v>
@@ -1820,11 +1824,11 @@
       <c r="H14" s="6"/>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1833,11 +1837,11 @@
       <c r="H15" s="6"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
         <v>45</v>
@@ -1848,11 +1852,11 @@
       <c r="H16" s="6"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="5" t="s">
         <v>45</v>
       </c>
@@ -1867,11 +1871,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="7" t="s">
         <v>45</v>
       </c>
@@ -1888,6 +1892,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
@@ -1904,15 +1916,8 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Matrices de trazabilidad modificadas en base a cambios en requisitos
</commit_message>
<xml_diff>
--- a/documentacion/matriz_de_trazabilidad_RI.xlsx
+++ b/documentacion/matriz_de_trazabilidad_RI.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17139420-B4FE-4BB5-B57B-99784BF7AFE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C8588-3836-5A4B-BB18-6BAB3491A057}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="54">
   <si>
     <t>Actividad</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Donación</t>
   </si>
   <si>
-    <t>Donante</t>
-  </si>
-  <si>
     <t>Evento</t>
   </si>
   <si>
@@ -80,45 +77,18 @@
     <t>Tutor Legal</t>
   </si>
   <si>
-    <t>Valoración</t>
-  </si>
-  <si>
     <t>Voluntario</t>
   </si>
   <si>
     <t>A                           RI</t>
   </si>
   <si>
-    <t>RI-001</t>
-  </si>
-  <si>
-    <t>RI-002</t>
-  </si>
-  <si>
-    <t>RI-003</t>
-  </si>
-  <si>
-    <t>RI-004</t>
-  </si>
-  <si>
-    <t>RI-005</t>
-  </si>
-  <si>
-    <t>RI-006</t>
-  </si>
-  <si>
-    <t>RI-007</t>
-  </si>
-  <si>
     <t>acompañaA</t>
   </si>
   <si>
     <t>colaboraEn</t>
   </si>
   <si>
-    <t>crea</t>
-  </si>
-  <si>
     <t>determina</t>
   </si>
   <si>
@@ -161,7 +131,58 @@
     <t>✔</t>
   </si>
   <si>
-    <t>C                           RI</t>
+    <t>Institución</t>
+  </si>
+  <si>
+    <t>C                          RI</t>
+  </si>
+  <si>
+    <t>RI-1</t>
+  </si>
+  <si>
+    <t>RI-2</t>
+  </si>
+  <si>
+    <t>RI-3</t>
+  </si>
+  <si>
+    <t>RI-4</t>
+  </si>
+  <si>
+    <t>RI-5</t>
+  </si>
+  <si>
+    <t>RI-6</t>
+  </si>
+  <si>
+    <t>RI-7</t>
+  </si>
+  <si>
+    <t>RI-8</t>
+  </si>
+  <si>
+    <t>RI-9</t>
+  </si>
+  <si>
+    <t>RI-10</t>
+  </si>
+  <si>
+    <t>RI-11</t>
+  </si>
+  <si>
+    <t>RI-12</t>
+  </si>
+  <si>
+    <t>presenta</t>
+  </si>
+  <si>
+    <t>cubre</t>
+  </si>
+  <si>
+    <t>encargadoDe</t>
+  </si>
+  <si>
+    <t>respondeA</t>
   </si>
 </sst>
 </file>
@@ -185,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -474,19 +495,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -546,21 +554,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -641,19 +634,6 @@
         <color auto="1"/>
       </diagonal>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
     <border diagonalDown="1">
       <left style="medium">
         <color indexed="64"/>
@@ -739,63 +719,261 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -804,40 +982,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -846,40 +1030,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1162,436 +1352,519 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="9" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="14" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="G3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="18"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="14" t="s">
-        <v>45</v>
-      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="I6" s="17"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="19"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="I7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="20"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="20"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="20"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="I10" s="17"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="20"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="D11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="23"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="20"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="29"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="19"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="27"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="19"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="27"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="23"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="29"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="5" t="s">
-        <v>45</v>
+      <c r="I15" s="17"/>
+      <c r="J15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="20"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="20"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="29"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="23"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="31"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="F18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="19"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="20"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="33"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="20"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="19"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="33"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="20"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="33"/>
-      <c r="C22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I23" s="17"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="33">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1600,322 +1873,530 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="14" width="7.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="41"/>
+      <c r="L1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="51"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="33"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="43"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="19"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="29"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="23"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="29"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="5"/>
+      <c r="I7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="53"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="10"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="23"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="27"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="37"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="29"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="23"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="45"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="19"/>
+      <c r="I13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="29"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="33"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="29"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="33"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="27"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="12"/>
+      <c r="H17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="53"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="55"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E24" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
+  <mergeCells count="32">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Tercera entrega finalizada y testeada
</commit_message>
<xml_diff>
--- a/documentacion/matriz_de_trazabilidad_RI.xlsx
+++ b/documentacion/matriz_de_trazabilidad_RI.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C8588-3836-5A4B-BB18-6BAB3491A057}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{73F2726A-7111-4C79-86E8-ED61FF2666B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Clases" sheetId="1" r:id="rId1"/>
+    <sheet name="Asociaciones" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
   <si>
     <t>Actividad</t>
   </si>
@@ -32,21 +32,12 @@
     <t>Cuestionario</t>
   </si>
   <si>
-    <t>Disponibilidad</t>
-  </si>
-  <si>
     <t>Donación</t>
   </si>
   <si>
     <t>Evento</t>
   </si>
   <si>
-    <t>Factura</t>
-  </si>
-  <si>
-    <t>Financiación</t>
-  </si>
-  <si>
     <t>Informe Médico</t>
   </si>
   <si>
@@ -89,21 +80,12 @@
     <t>colaboraEn</t>
   </si>
   <si>
-    <t>determina</t>
-  </si>
-  <si>
     <t>donadoEn</t>
   </si>
   <si>
-    <t>elabora</t>
-  </si>
-  <si>
     <t>envía</t>
   </si>
   <si>
-    <t>financia</t>
-  </si>
-  <si>
     <t>genera</t>
   </si>
   <si>
@@ -113,9 +95,6 @@
     <t>paga</t>
   </si>
   <si>
-    <t>realiza</t>
-  </si>
-  <si>
     <t>recibe</t>
   </si>
   <si>
@@ -173,16 +152,28 @@
     <t>RI-12</t>
   </si>
   <si>
-    <t>presenta</t>
-  </si>
-  <si>
-    <t>cubre</t>
-  </si>
-  <si>
     <t>encargadoDe</t>
   </si>
   <si>
-    <t>respondeA</t>
+    <t>Recibo</t>
+  </si>
+  <si>
+    <t>Patrocinio</t>
+  </si>
+  <si>
+    <t>patrocina</t>
+  </si>
+  <si>
+    <t>estaInteresadoEn</t>
+  </si>
+  <si>
+    <t>seInscribe</t>
+  </si>
+  <si>
+    <t>responde</t>
+  </si>
+  <si>
+    <t>formula</t>
   </si>
 </sst>
 </file>
@@ -206,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -791,17 +782,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -881,17 +861,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -899,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -958,22 +927,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -982,47 +987,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1030,47 +1026,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1352,87 +1315,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A3" sqref="A3:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="14" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="14" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="25" t="s">
+      <c r="J1" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="K1" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="L1" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="M1" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="N1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="35"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="41"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="15"/>
@@ -1442,13 +1405,13 @@
       <c r="M3" s="4"/>
       <c r="N3" s="16"/>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1462,11 +1425,11 @@
       <c r="M4" s="6"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="12"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1479,32 +1442,30 @@
       <c r="L5" s="6"/>
       <c r="M5" s="17"/>
       <c r="N5" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="19"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
@@ -1512,29 +1473,29 @@
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="I7" s="17"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="20"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="17"/>
@@ -1542,13 +1503,13 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="20"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="29"/>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="27"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1556,19 +1517,19 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="17"/>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K9" s="6"/>
-      <c r="L9" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="20"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="29"/>
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="39"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1577,21 +1538,21 @@
       <c r="H10" s="6"/>
       <c r="I10" s="17"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="20"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="29"/>
+      <c r="M10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="39"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1602,13 +1563,13 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="20"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="29"/>
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="27"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1617,16 +1578,16 @@
       <c r="H12" s="6"/>
       <c r="I12" s="17"/>
       <c r="J12" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="20"/>
-    </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="5"/>
@@ -1637,38 +1598,46 @@
       <c r="H13" s="6"/>
       <c r="I13" s="17"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" s="20"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="5"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="17"/>
+      <c r="H14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="20"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="29"/>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="27"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1676,49 +1645,45 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="20"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="6"/>
+      <c r="N15" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="H16" s="6"/>
       <c r="I16" s="17"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="20"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="19"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="17"/>
@@ -1726,41 +1691,37 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="31"/>
+      <c r="N17" s="19"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="27"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="17"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="L18" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="M18" s="6"/>
-      <c r="N18" s="20"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="33"/>
+      <c r="N18" s="19"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="43"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="17"/>
@@ -1768,103 +1729,84 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="20"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="31"/>
+      <c r="N19" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="29"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="I20" s="17"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="20"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="22"/>
+      <c r="N20" s="19"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:B2"/>
+  <mergeCells count="32">
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1873,86 +1815,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A3" sqref="A3:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="14" width="7.33203125" customWidth="1"/>
+    <col min="3" max="14" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="25" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="K1" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="L1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="M1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="N1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="35"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="41"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="51"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="50"/>
       <c r="C3" s="1"/>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1964,19 +1906,19 @@
       <c r="M3" s="2"/>
       <c r="N3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="43"/>
+    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="52"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1986,41 +1928,39 @@
       <c r="M4" s="4"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="29"/>
+    <row r="5" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="27"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="J5" s="6"/>
-      <c r="K5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="6"/>
-      <c r="N5" s="11"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="6"/>
+      <c r="N5" s="22"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2028,63 +1968,63 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="11"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="5"/>
+      <c r="N6" s="10"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="53"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="M7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2092,293 +2032,255 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="10"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" s="27"/>
-      <c r="C10" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="L10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="6"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="27"/>
+    <row r="11" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="55"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="I11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="29"/>
+    <row r="12" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="27"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="45"/>
+    <row r="13" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="39"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="29"/>
+    <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="52"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K14" s="6"/>
-      <c r="L14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="29"/>
+    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="52"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="11"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="22"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="11"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="43"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="27"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="M17" s="17"/>
       <c r="N17" s="11"/>
     </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="43"/>
+    <row r="18" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="29"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="53"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="55"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="56" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E24" s="57"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E22" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="A7:B7"/>
+  <mergeCells count="30">
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
@@ -2386,17 +2288,17 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>